<commit_message>
Merged in issue#204-conditional-formatting-order (pull request #140)
issue#204 - add conditional formatting rules according to the original rule priority

* issue#204 - add conditional formatting rules according to the original rule priority

* issue#204 - reverted change of TestWorkbook.java because getCellStyle()

    isn't used.

Approved-by: Marcus Warm <marcus.warm@x-map.de>
</commit_message>
<xml_diff>
--- a/jxls-poi/src/test/resources/org/jxls/templatebasedtests/ConditionalFormattingTest.xlsx
+++ b/jxls-poi/src/test/resources/org/jxls/templatebasedtests/ConditionalFormattingTest.xlsx
@@ -172,11 +172,22 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -486,7 +497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -516,12 +529,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
+      <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:B3">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>